<commit_message>
changed user manual(added images)
</commit_message>
<xml_diff>
--- a/output/final_gen.xlsx
+++ b/output/final_gen.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E109"/>
+  <dimension ref="A1:E163"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -1601,10 +1601,8 @@
       <c r="B56" t="n">
         <v>0</v>
       </c>
-      <c r="C56" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C56" t="n">
+        <v>0</v>
       </c>
       <c r="D56" t="inlineStr">
         <is>
@@ -1624,10 +1622,8 @@
       <c r="B57" t="n">
         <v>0</v>
       </c>
-      <c r="C57" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C57" t="n">
+        <v>1</v>
       </c>
       <c r="D57" t="inlineStr">
         <is>
@@ -1647,10 +1643,8 @@
       <c r="B58" t="n">
         <v>0</v>
       </c>
-      <c r="C58" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="C58" t="n">
+        <v>2</v>
       </c>
       <c r="D58" t="inlineStr">
         <is>
@@ -1670,10 +1664,8 @@
       <c r="B59" t="n">
         <v>0</v>
       </c>
-      <c r="C59" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="C59" t="n">
+        <v>3</v>
       </c>
       <c r="D59" t="inlineStr">
         <is>
@@ -1693,10 +1685,8 @@
       <c r="B60" t="n">
         <v>0</v>
       </c>
-      <c r="C60" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="C60" t="n">
+        <v>4</v>
       </c>
       <c r="D60" t="inlineStr">
         <is>
@@ -1716,10 +1706,8 @@
       <c r="B61" t="n">
         <v>0</v>
       </c>
-      <c r="C61" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="C61" t="n">
+        <v>5</v>
       </c>
       <c r="D61" t="inlineStr">
         <is>
@@ -1739,10 +1727,8 @@
       <c r="B62" t="n">
         <v>0</v>
       </c>
-      <c r="C62" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="C62" t="n">
+        <v>6</v>
       </c>
       <c r="D62" t="inlineStr">
         <is>
@@ -1762,10 +1748,8 @@
       <c r="B63" t="n">
         <v>0</v>
       </c>
-      <c r="C63" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="C63" t="n">
+        <v>7</v>
       </c>
       <c r="D63" t="inlineStr">
         <is>
@@ -1785,10 +1769,8 @@
       <c r="B64" t="n">
         <v>0</v>
       </c>
-      <c r="C64" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="C64" t="n">
+        <v>8</v>
       </c>
       <c r="D64" t="inlineStr">
         <is>
@@ -1808,10 +1790,8 @@
       <c r="B65" t="n">
         <v>0</v>
       </c>
-      <c r="C65" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="C65" t="n">
+        <v>9</v>
       </c>
       <c r="D65" t="inlineStr">
         <is>
@@ -1831,10 +1811,8 @@
       <c r="B66" t="n">
         <v>0</v>
       </c>
-      <c r="C66" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="C66" t="n">
+        <v>10</v>
       </c>
       <c r="D66" t="inlineStr">
         <is>
@@ -1854,10 +1832,8 @@
       <c r="B67" t="n">
         <v>0</v>
       </c>
-      <c r="C67" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="C67" t="n">
+        <v>11</v>
       </c>
       <c r="D67" t="inlineStr">
         <is>
@@ -1877,10 +1853,8 @@
       <c r="B68" t="n">
         <v>0</v>
       </c>
-      <c r="C68" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="C68" t="n">
+        <v>12</v>
       </c>
       <c r="D68" t="inlineStr">
         <is>
@@ -1900,10 +1874,8 @@
       <c r="B69" t="n">
         <v>1</v>
       </c>
-      <c r="C69" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C69" t="n">
+        <v>0</v>
       </c>
       <c r="D69" t="inlineStr">
         <is>
@@ -1923,10 +1895,8 @@
       <c r="B70" t="n">
         <v>1</v>
       </c>
-      <c r="C70" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C70" t="n">
+        <v>1</v>
       </c>
       <c r="D70" t="inlineStr">
         <is>
@@ -1946,10 +1916,8 @@
       <c r="B71" t="n">
         <v>1</v>
       </c>
-      <c r="C71" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="C71" t="n">
+        <v>2</v>
       </c>
       <c r="D71" t="inlineStr">
         <is>
@@ -1969,10 +1937,8 @@
       <c r="B72" t="n">
         <v>1</v>
       </c>
-      <c r="C72" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="C72" t="n">
+        <v>3</v>
       </c>
       <c r="D72" t="inlineStr">
         <is>
@@ -1992,10 +1958,8 @@
       <c r="B73" t="n">
         <v>1</v>
       </c>
-      <c r="C73" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="C73" t="n">
+        <v>4</v>
       </c>
       <c r="D73" t="inlineStr">
         <is>
@@ -2015,10 +1979,8 @@
       <c r="B74" t="n">
         <v>1</v>
       </c>
-      <c r="C74" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="C74" t="n">
+        <v>5</v>
       </c>
       <c r="D74" t="inlineStr">
         <is>
@@ -2038,10 +2000,8 @@
       <c r="B75" t="n">
         <v>1</v>
       </c>
-      <c r="C75" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="C75" t="n">
+        <v>6</v>
       </c>
       <c r="D75" t="inlineStr">
         <is>
@@ -2061,10 +2021,8 @@
       <c r="B76" t="n">
         <v>1</v>
       </c>
-      <c r="C76" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="C76" t="n">
+        <v>7</v>
       </c>
       <c r="D76" t="inlineStr">
         <is>
@@ -2084,10 +2042,8 @@
       <c r="B77" t="n">
         <v>1</v>
       </c>
-      <c r="C77" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="C77" t="n">
+        <v>8</v>
       </c>
       <c r="D77" t="inlineStr">
         <is>
@@ -2107,10 +2063,8 @@
       <c r="B78" t="n">
         <v>1</v>
       </c>
-      <c r="C78" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="C78" t="n">
+        <v>9</v>
       </c>
       <c r="D78" t="inlineStr">
         <is>
@@ -2130,10 +2084,8 @@
       <c r="B79" t="n">
         <v>1</v>
       </c>
-      <c r="C79" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="C79" t="n">
+        <v>10</v>
       </c>
       <c r="D79" t="inlineStr">
         <is>
@@ -2153,10 +2105,8 @@
       <c r="B80" t="n">
         <v>1</v>
       </c>
-      <c r="C80" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="C80" t="n">
+        <v>11</v>
       </c>
       <c r="D80" t="inlineStr">
         <is>
@@ -2176,10 +2126,8 @@
       <c r="B81" t="n">
         <v>1</v>
       </c>
-      <c r="C81" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="C81" t="n">
+        <v>12</v>
       </c>
       <c r="D81" t="inlineStr">
         <is>
@@ -2199,10 +2147,8 @@
       <c r="B82" t="n">
         <v>1</v>
       </c>
-      <c r="C82" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="C82" t="n">
+        <v>13</v>
       </c>
       <c r="D82" t="inlineStr">
         <is>
@@ -2222,10 +2168,8 @@
       <c r="B83" t="n">
         <v>1</v>
       </c>
-      <c r="C83" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="C83" t="n">
+        <v>14</v>
       </c>
       <c r="D83" t="inlineStr">
         <is>
@@ -2245,10 +2189,8 @@
       <c r="B84" t="n">
         <v>1</v>
       </c>
-      <c r="C84" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="C84" t="n">
+        <v>15</v>
       </c>
       <c r="D84" t="inlineStr">
         <is>
@@ -2268,10 +2210,8 @@
       <c r="B85" t="n">
         <v>1</v>
       </c>
-      <c r="C85" t="inlineStr">
-        <is>
-          <t>16</t>
-        </is>
+      <c r="C85" t="n">
+        <v>16</v>
       </c>
       <c r="D85" t="inlineStr">
         <is>
@@ -2291,10 +2231,8 @@
       <c r="B86" t="n">
         <v>1</v>
       </c>
-      <c r="C86" t="inlineStr">
-        <is>
-          <t>17</t>
-        </is>
+      <c r="C86" t="n">
+        <v>17</v>
       </c>
       <c r="D86" t="inlineStr">
         <is>
@@ -2314,10 +2252,8 @@
       <c r="B87" t="n">
         <v>1</v>
       </c>
-      <c r="C87" t="inlineStr">
-        <is>
-          <t>18</t>
-        </is>
+      <c r="C87" t="n">
+        <v>18</v>
       </c>
       <c r="D87" t="inlineStr">
         <is>
@@ -2337,10 +2273,8 @@
       <c r="B88" t="n">
         <v>1</v>
       </c>
-      <c r="C88" t="inlineStr">
-        <is>
-          <t>19</t>
-        </is>
+      <c r="C88" t="n">
+        <v>19</v>
       </c>
       <c r="D88" t="inlineStr">
         <is>
@@ -2360,10 +2294,8 @@
       <c r="B89" t="n">
         <v>1</v>
       </c>
-      <c r="C89" t="inlineStr">
-        <is>
-          <t>20</t>
-        </is>
+      <c r="C89" t="n">
+        <v>20</v>
       </c>
       <c r="D89" t="inlineStr">
         <is>
@@ -2383,10 +2315,8 @@
       <c r="B90" t="n">
         <v>1</v>
       </c>
-      <c r="C90" t="inlineStr">
-        <is>
-          <t>21</t>
-        </is>
+      <c r="C90" t="n">
+        <v>21</v>
       </c>
       <c r="D90" t="inlineStr">
         <is>
@@ -2406,10 +2336,8 @@
       <c r="B91" t="n">
         <v>1</v>
       </c>
-      <c r="C91" t="inlineStr">
-        <is>
-          <t>22</t>
-        </is>
+      <c r="C91" t="n">
+        <v>22</v>
       </c>
       <c r="D91" t="inlineStr">
         <is>
@@ -2429,10 +2357,8 @@
       <c r="B92" t="n">
         <v>1</v>
       </c>
-      <c r="C92" t="inlineStr">
-        <is>
-          <t>23</t>
-        </is>
+      <c r="C92" t="n">
+        <v>23</v>
       </c>
       <c r="D92" t="inlineStr">
         <is>
@@ -2452,10 +2378,8 @@
       <c r="B93" t="n">
         <v>2</v>
       </c>
-      <c r="C93" t="inlineStr">
-        <is>
-          <t>0</t>
-        </is>
+      <c r="C93" t="n">
+        <v>0</v>
       </c>
       <c r="D93" t="inlineStr">
         <is>
@@ -2475,10 +2399,8 @@
       <c r="B94" t="n">
         <v>2</v>
       </c>
-      <c r="C94" t="inlineStr">
-        <is>
-          <t>1</t>
-        </is>
+      <c r="C94" t="n">
+        <v>1</v>
       </c>
       <c r="D94" t="inlineStr">
         <is>
@@ -2498,10 +2420,8 @@
       <c r="B95" t="n">
         <v>2</v>
       </c>
-      <c r="C95" t="inlineStr">
-        <is>
-          <t>2</t>
-        </is>
+      <c r="C95" t="n">
+        <v>2</v>
       </c>
       <c r="D95" t="inlineStr">
         <is>
@@ -2521,10 +2441,8 @@
       <c r="B96" t="n">
         <v>2</v>
       </c>
-      <c r="C96" t="inlineStr">
-        <is>
-          <t>3</t>
-        </is>
+      <c r="C96" t="n">
+        <v>3</v>
       </c>
       <c r="D96" t="inlineStr">
         <is>
@@ -2544,10 +2462,8 @@
       <c r="B97" t="n">
         <v>2</v>
       </c>
-      <c r="C97" t="inlineStr">
-        <is>
-          <t>4</t>
-        </is>
+      <c r="C97" t="n">
+        <v>4</v>
       </c>
       <c r="D97" t="inlineStr">
         <is>
@@ -2567,10 +2483,8 @@
       <c r="B98" t="n">
         <v>2</v>
       </c>
-      <c r="C98" t="inlineStr">
-        <is>
-          <t>5</t>
-        </is>
+      <c r="C98" t="n">
+        <v>5</v>
       </c>
       <c r="D98" t="inlineStr">
         <is>
@@ -2590,10 +2504,8 @@
       <c r="B99" t="n">
         <v>2</v>
       </c>
-      <c r="C99" t="inlineStr">
-        <is>
-          <t>6</t>
-        </is>
+      <c r="C99" t="n">
+        <v>6</v>
       </c>
       <c r="D99" t="inlineStr">
         <is>
@@ -2613,10 +2525,8 @@
       <c r="B100" t="n">
         <v>2</v>
       </c>
-      <c r="C100" t="inlineStr">
-        <is>
-          <t>7</t>
-        </is>
+      <c r="C100" t="n">
+        <v>7</v>
       </c>
       <c r="D100" t="inlineStr">
         <is>
@@ -2636,10 +2546,8 @@
       <c r="B101" t="n">
         <v>2</v>
       </c>
-      <c r="C101" t="inlineStr">
-        <is>
-          <t>8</t>
-        </is>
+      <c r="C101" t="n">
+        <v>8</v>
       </c>
       <c r="D101" t="inlineStr">
         <is>
@@ -2659,10 +2567,8 @@
       <c r="B102" t="n">
         <v>2</v>
       </c>
-      <c r="C102" t="inlineStr">
-        <is>
-          <t>9</t>
-        </is>
+      <c r="C102" t="n">
+        <v>9</v>
       </c>
       <c r="D102" t="inlineStr">
         <is>
@@ -2682,10 +2588,8 @@
       <c r="B103" t="n">
         <v>2</v>
       </c>
-      <c r="C103" t="inlineStr">
-        <is>
-          <t>10</t>
-        </is>
+      <c r="C103" t="n">
+        <v>10</v>
       </c>
       <c r="D103" t="inlineStr">
         <is>
@@ -2705,10 +2609,8 @@
       <c r="B104" t="n">
         <v>2</v>
       </c>
-      <c r="C104" t="inlineStr">
-        <is>
-          <t>11</t>
-        </is>
+      <c r="C104" t="n">
+        <v>11</v>
       </c>
       <c r="D104" t="inlineStr">
         <is>
@@ -2728,10 +2630,8 @@
       <c r="B105" t="n">
         <v>2</v>
       </c>
-      <c r="C105" t="inlineStr">
-        <is>
-          <t>12</t>
-        </is>
+      <c r="C105" t="n">
+        <v>12</v>
       </c>
       <c r="D105" t="inlineStr">
         <is>
@@ -2751,10 +2651,8 @@
       <c r="B106" t="n">
         <v>2</v>
       </c>
-      <c r="C106" t="inlineStr">
-        <is>
-          <t>13</t>
-        </is>
+      <c r="C106" t="n">
+        <v>13</v>
       </c>
       <c r="D106" t="inlineStr">
         <is>
@@ -2774,10 +2672,8 @@
       <c r="B107" t="n">
         <v>2</v>
       </c>
-      <c r="C107" t="inlineStr">
-        <is>
-          <t>14</t>
-        </is>
+      <c r="C107" t="n">
+        <v>14</v>
       </c>
       <c r="D107" t="inlineStr">
         <is>
@@ -2797,10 +2693,8 @@
       <c r="B108" t="n">
         <v>2</v>
       </c>
-      <c r="C108" t="inlineStr">
-        <is>
-          <t>15</t>
-        </is>
+      <c r="C108" t="n">
+        <v>15</v>
       </c>
       <c r="D108" t="inlineStr">
         <is>
@@ -2820,17 +2714,1257 @@
       <c r="B109" t="n">
         <v>2</v>
       </c>
-      <c r="C109" t="inlineStr">
+      <c r="C109" t="n">
+        <v>16</v>
+      </c>
+      <c r="D109" t="inlineStr">
+        <is>
+          <t>way</t>
+        </is>
+      </c>
+      <c r="E109" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="110">
+      <c r="A110" t="n">
+        <v>0</v>
+      </c>
+      <c r="B110" t="n">
+        <v>0</v>
+      </c>
+      <c r="C110" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D110" t="inlineStr">
+        <is>
+          <t>On</t>
+        </is>
+      </c>
+      <c r="E110" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="111">
+      <c r="A111" t="n">
+        <v>0</v>
+      </c>
+      <c r="B111" t="n">
+        <v>0</v>
+      </c>
+      <c r="C111" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D111" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+      <c r="E111" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="112">
+      <c r="A112" t="n">
+        <v>0</v>
+      </c>
+      <c r="B112" t="n">
+        <v>0</v>
+      </c>
+      <c r="C112" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D112" t="inlineStr">
+        <is>
+          <t>edge</t>
+        </is>
+      </c>
+      <c r="E112" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="113">
+      <c r="A113" t="n">
+        <v>0</v>
+      </c>
+      <c r="B113" t="n">
+        <v>0</v>
+      </c>
+      <c r="C113" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D113" t="inlineStr">
+        <is>
+          <t>of</t>
+        </is>
+      </c>
+      <c r="E113" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="114">
+      <c r="A114" t="n">
+        <v>0</v>
+      </c>
+      <c r="B114" t="n">
+        <v>0</v>
+      </c>
+      <c r="C114" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D114" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E114" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="115">
+      <c r="A115" t="n">
+        <v>0</v>
+      </c>
+      <c r="B115" t="n">
+        <v>0</v>
+      </c>
+      <c r="C115" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D115" t="inlineStr">
+        <is>
+          <t>small,</t>
+        </is>
+      </c>
+      <c r="E115" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="116">
+      <c r="A116" t="n">
+        <v>0</v>
+      </c>
+      <c r="B116" t="n">
+        <v>0</v>
+      </c>
+      <c r="C116" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D116" t="inlineStr">
+        <is>
+          <t>misty</t>
+        </is>
+      </c>
+      <c r="E116" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="117">
+      <c r="A117" t="n">
+        <v>0</v>
+      </c>
+      <c r="B117" t="n">
+        <v>0</v>
+      </c>
+      <c r="C117" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D117" t="inlineStr">
+        <is>
+          <t>island</t>
+        </is>
+      </c>
+      <c r="E117" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="118">
+      <c r="A118" t="n">
+        <v>0</v>
+      </c>
+      <c r="B118" t="n">
+        <v>0</v>
+      </c>
+      <c r="C118" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D118" t="inlineStr">
+        <is>
+          <t>stood</t>
+        </is>
+      </c>
+      <c r="E118" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="119">
+      <c r="A119" t="n">
+        <v>0</v>
+      </c>
+      <c r="B119" t="n">
+        <v>0</v>
+      </c>
+      <c r="C119" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D119" t="inlineStr">
+        <is>
+          <t>little</t>
+        </is>
+      </c>
+      <c r="E119" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="120">
+      <c r="A120" t="n">
+        <v>0</v>
+      </c>
+      <c r="B120" t="n">
+        <v>0</v>
+      </c>
+      <c r="C120" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D120" t="inlineStr">
+        <is>
+          <t>lighthouse</t>
+        </is>
+      </c>
+      <c r="E120" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="121">
+      <c r="A121" t="n">
+        <v>0</v>
+      </c>
+      <c r="B121" t="n">
+        <v>0</v>
+      </c>
+      <c r="C121" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D121" t="inlineStr">
+        <is>
+          <t>named</t>
+        </is>
+      </c>
+      <c r="E121" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="122">
+      <c r="A122" t="n">
+        <v>0</v>
+      </c>
+      <c r="B122" t="n">
+        <v>0</v>
+      </c>
+      <c r="C122" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D122" t="inlineStr">
+        <is>
+          <t>Lumy</t>
+        </is>
+      </c>
+      <c r="E122" t="inlineStr">
+        <is>
+          <t>B-PER</t>
+        </is>
+      </c>
+    </row>
+    <row r="123">
+      <c r="A123" t="n">
+        <v>0</v>
+      </c>
+      <c r="B123" t="n">
+        <v>1</v>
+      </c>
+      <c r="C123" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D123" t="inlineStr">
+        <is>
+          <t>Unlike</t>
+        </is>
+      </c>
+      <c r="E123" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="124">
+      <c r="A124" t="n">
+        <v>0</v>
+      </c>
+      <c r="B124" t="n">
+        <v>1</v>
+      </c>
+      <c r="C124" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D124" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+      <c r="E124" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="125">
+      <c r="A125" t="n">
+        <v>0</v>
+      </c>
+      <c r="B125" t="n">
+        <v>1</v>
+      </c>
+      <c r="C125" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D125" t="inlineStr">
+        <is>
+          <t>towering</t>
+        </is>
+      </c>
+      <c r="E125" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="126">
+      <c r="A126" t="n">
+        <v>0</v>
+      </c>
+      <c r="B126" t="n">
+        <v>1</v>
+      </c>
+      <c r="C126" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D126" t="inlineStr">
+        <is>
+          <t>lighthouses</t>
+        </is>
+      </c>
+      <c r="E126" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="127">
+      <c r="A127" t="n">
+        <v>0</v>
+      </c>
+      <c r="B127" t="n">
+        <v>1</v>
+      </c>
+      <c r="C127" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D127" t="inlineStr">
+        <is>
+          <t>that</t>
+        </is>
+      </c>
+      <c r="E127" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="128">
+      <c r="A128" t="n">
+        <v>0</v>
+      </c>
+      <c r="B128" t="n">
+        <v>1</v>
+      </c>
+      <c r="C128" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D128" t="inlineStr">
+        <is>
+          <t>stretched</t>
+        </is>
+      </c>
+      <c r="E128" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="129">
+      <c r="A129" t="n">
+        <v>0</v>
+      </c>
+      <c r="B129" t="n">
+        <v>1</v>
+      </c>
+      <c r="C129" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D129" t="inlineStr">
+        <is>
+          <t>into</t>
+        </is>
+      </c>
+      <c r="E129" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="130">
+      <c r="A130" t="n">
+        <v>0</v>
+      </c>
+      <c r="B130" t="n">
+        <v>1</v>
+      </c>
+      <c r="C130" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D130" t="inlineStr">
+        <is>
+          <t>clouds,</t>
+        </is>
+      </c>
+      <c r="E130" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="131">
+      <c r="A131" t="n">
+        <v>0</v>
+      </c>
+      <c r="B131" t="n">
+        <v>1</v>
+      </c>
+      <c r="C131" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D131" t="inlineStr">
+        <is>
+          <t>Lumy</t>
+        </is>
+      </c>
+      <c r="E131" t="inlineStr">
+        <is>
+          <t>B-PER</t>
+        </is>
+      </c>
+    </row>
+    <row r="132">
+      <c r="A132" t="n">
+        <v>0</v>
+      </c>
+      <c r="B132" t="n">
+        <v>1</v>
+      </c>
+      <c r="C132" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D132" t="inlineStr">
+        <is>
+          <t>was</t>
+        </is>
+      </c>
+      <c r="E132" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="133">
+      <c r="A133" t="n">
+        <v>0</v>
+      </c>
+      <c r="B133" t="n">
+        <v>1</v>
+      </c>
+      <c r="C133" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D133" t="inlineStr">
+        <is>
+          <t>small</t>
+        </is>
+      </c>
+      <c r="E133" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="134">
+      <c r="A134" t="n">
+        <v>0</v>
+      </c>
+      <c r="B134" t="n">
+        <v>1</v>
+      </c>
+      <c r="C134" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D134" t="inlineStr">
+        <is>
+          <t>and</t>
+        </is>
+      </c>
+      <c r="E134" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="135">
+      <c r="A135" t="n">
+        <v>0</v>
+      </c>
+      <c r="B135" t="n">
+        <v>1</v>
+      </c>
+      <c r="C135" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D135" t="inlineStr">
+        <is>
+          <t>a</t>
+        </is>
+      </c>
+      <c r="E135" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="136">
+      <c r="A136" t="n">
+        <v>0</v>
+      </c>
+      <c r="B136" t="n">
+        <v>1</v>
+      </c>
+      <c r="C136" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D136" t="inlineStr">
+        <is>
+          <t>bit</t>
+        </is>
+      </c>
+      <c r="E136" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="137">
+      <c r="A137" t="n">
+        <v>0</v>
+      </c>
+      <c r="B137" t="n">
+        <v>1</v>
+      </c>
+      <c r="C137" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D137" t="inlineStr">
+        <is>
+          <t>crooked,</t>
+        </is>
+      </c>
+      <c r="E137" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="138">
+      <c r="A138" t="n">
+        <v>0</v>
+      </c>
+      <c r="B138" t="n">
+        <v>1</v>
+      </c>
+      <c r="C138" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D138" t="inlineStr">
+        <is>
+          <t>with</t>
+        </is>
+      </c>
+      <c r="E138" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="139">
+      <c r="A139" t="n">
+        <v>0</v>
+      </c>
+      <c r="B139" t="n">
+        <v>1</v>
+      </c>
+      <c r="C139" t="inlineStr">
         <is>
           <t>16</t>
         </is>
       </c>
-      <c r="D109" t="inlineStr">
+      <c r="D139" t="inlineStr">
+        <is>
+          <t>its</t>
+        </is>
+      </c>
+      <c r="E139" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="140">
+      <c r="A140" t="n">
+        <v>0</v>
+      </c>
+      <c r="B140" t="n">
+        <v>1</v>
+      </c>
+      <c r="C140" t="inlineStr">
+        <is>
+          <t>17</t>
+        </is>
+      </c>
+      <c r="D140" t="inlineStr">
+        <is>
+          <t>paint</t>
+        </is>
+      </c>
+      <c r="E140" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="141">
+      <c r="A141" t="n">
+        <v>0</v>
+      </c>
+      <c r="B141" t="n">
+        <v>1</v>
+      </c>
+      <c r="C141" t="inlineStr">
+        <is>
+          <t>18</t>
+        </is>
+      </c>
+      <c r="D141" t="inlineStr">
+        <is>
+          <t>chipped</t>
+        </is>
+      </c>
+      <c r="E141" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="142">
+      <c r="A142" t="n">
+        <v>0</v>
+      </c>
+      <c r="B142" t="n">
+        <v>1</v>
+      </c>
+      <c r="C142" t="inlineStr">
+        <is>
+          <t>19</t>
+        </is>
+      </c>
+      <c r="D142" t="inlineStr">
+        <is>
+          <t>light</t>
+        </is>
+      </c>
+      <c r="E142" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="143">
+      <c r="A143" t="n">
+        <v>0</v>
+      </c>
+      <c r="B143" t="n">
+        <v>1</v>
+      </c>
+      <c r="C143" t="inlineStr">
+        <is>
+          <t>20</t>
+        </is>
+      </c>
+      <c r="D143" t="inlineStr">
+        <is>
+          <t>not</t>
+        </is>
+      </c>
+      <c r="E143" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="144">
+      <c r="A144" t="n">
+        <v>0</v>
+      </c>
+      <c r="B144" t="n">
+        <v>1</v>
+      </c>
+      <c r="C144" t="inlineStr">
+        <is>
+          <t>21</t>
+        </is>
+      </c>
+      <c r="D144" t="inlineStr">
+        <is>
+          <t>as</t>
+        </is>
+      </c>
+      <c r="E144" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="145">
+      <c r="A145" t="n">
+        <v>0</v>
+      </c>
+      <c r="B145" t="n">
+        <v>1</v>
+      </c>
+      <c r="C145" t="inlineStr">
+        <is>
+          <t>22</t>
+        </is>
+      </c>
+      <c r="D145" t="inlineStr">
+        <is>
+          <t>bright</t>
+        </is>
+      </c>
+      <c r="E145" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="146">
+      <c r="A146" t="n">
+        <v>0</v>
+      </c>
+      <c r="B146" t="n">
+        <v>1</v>
+      </c>
+      <c r="C146" t="inlineStr">
+        <is>
+          <t>23</t>
+        </is>
+      </c>
+      <c r="D146" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
+      <c r="E146" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="147">
+      <c r="A147" t="n">
+        <v>0</v>
+      </c>
+      <c r="B147" t="n">
+        <v>2</v>
+      </c>
+      <c r="C147" t="inlineStr">
+        <is>
+          <t>0</t>
+        </is>
+      </c>
+      <c r="D147" t="inlineStr">
+        <is>
+          <t>But</t>
+        </is>
+      </c>
+      <c r="E147" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="148">
+      <c r="A148" t="n">
+        <v>0</v>
+      </c>
+      <c r="B148" t="n">
+        <v>2</v>
+      </c>
+      <c r="C148" t="inlineStr">
+        <is>
+          <t>1</t>
+        </is>
+      </c>
+      <c r="D148" t="inlineStr">
+        <is>
+          <t>Lumy</t>
+        </is>
+      </c>
+      <c r="E148" t="inlineStr">
+        <is>
+          <t>B-PER</t>
+        </is>
+      </c>
+    </row>
+    <row r="149">
+      <c r="A149" t="n">
+        <v>0</v>
+      </c>
+      <c r="B149" t="n">
+        <v>2</v>
+      </c>
+      <c r="C149" t="inlineStr">
+        <is>
+          <t>2</t>
+        </is>
+      </c>
+      <c r="D149" t="inlineStr">
+        <is>
+          <t>had</t>
+        </is>
+      </c>
+      <c r="E149" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="150">
+      <c r="A150" t="n">
+        <v>0</v>
+      </c>
+      <c r="B150" t="n">
+        <v>2</v>
+      </c>
+      <c r="C150" t="inlineStr">
+        <is>
+          <t>3</t>
+        </is>
+      </c>
+      <c r="D150" t="inlineStr">
+        <is>
+          <t>one</t>
+        </is>
+      </c>
+      <c r="E150" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="151">
+      <c r="A151" t="n">
+        <v>0</v>
+      </c>
+      <c r="B151" t="n">
+        <v>2</v>
+      </c>
+      <c r="C151" t="inlineStr">
+        <is>
+          <t>4</t>
+        </is>
+      </c>
+      <c r="D151" t="inlineStr">
+        <is>
+          <t>thing</t>
+        </is>
+      </c>
+      <c r="E151" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="152">
+      <c r="A152" t="n">
+        <v>0</v>
+      </c>
+      <c r="B152" t="n">
+        <v>2</v>
+      </c>
+      <c r="C152" t="inlineStr">
+        <is>
+          <t>5</t>
+        </is>
+      </c>
+      <c r="D152" t="inlineStr">
+        <is>
+          <t>the</t>
+        </is>
+      </c>
+      <c r="E152" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="153">
+      <c r="A153" t="n">
+        <v>0</v>
+      </c>
+      <c r="B153" t="n">
+        <v>2</v>
+      </c>
+      <c r="C153" t="inlineStr">
+        <is>
+          <t>6</t>
+        </is>
+      </c>
+      <c r="D153" t="inlineStr">
+        <is>
+          <t>others</t>
+        </is>
+      </c>
+      <c r="E153" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="154">
+      <c r="A154" t="n">
+        <v>0</v>
+      </c>
+      <c r="B154" t="n">
+        <v>2</v>
+      </c>
+      <c r="C154" t="inlineStr">
+        <is>
+          <t>7</t>
+        </is>
+      </c>
+      <c r="D154" t="inlineStr">
+        <is>
+          <t>didnâ€™t:</t>
+        </is>
+      </c>
+      <c r="E154" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="155">
+      <c r="A155" t="n">
+        <v>0</v>
+      </c>
+      <c r="B155" t="n">
+        <v>2</v>
+      </c>
+      <c r="C155" t="inlineStr">
+        <is>
+          <t>8</t>
+        </is>
+      </c>
+      <c r="D155" t="inlineStr">
+        <is>
+          <t>an</t>
+        </is>
+      </c>
+      <c r="E155" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="156">
+      <c r="A156" t="n">
+        <v>0</v>
+      </c>
+      <c r="B156" t="n">
+        <v>2</v>
+      </c>
+      <c r="C156" t="inlineStr">
+        <is>
+          <t>9</t>
+        </is>
+      </c>
+      <c r="D156" t="inlineStr">
+        <is>
+          <t>unshakable</t>
+        </is>
+      </c>
+      <c r="E156" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="157">
+      <c r="A157" t="n">
+        <v>0</v>
+      </c>
+      <c r="B157" t="n">
+        <v>2</v>
+      </c>
+      <c r="C157" t="inlineStr">
+        <is>
+          <t>10</t>
+        </is>
+      </c>
+      <c r="D157" t="inlineStr">
+        <is>
+          <t>determination</t>
+        </is>
+      </c>
+      <c r="E157" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="158">
+      <c r="A158" t="n">
+        <v>0</v>
+      </c>
+      <c r="B158" t="n">
+        <v>2</v>
+      </c>
+      <c r="C158" t="inlineStr">
+        <is>
+          <t>11</t>
+        </is>
+      </c>
+      <c r="D158" t="inlineStr">
+        <is>
+          <t>to</t>
+        </is>
+      </c>
+      <c r="E158" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="159">
+      <c r="A159" t="n">
+        <v>0</v>
+      </c>
+      <c r="B159" t="n">
+        <v>2</v>
+      </c>
+      <c r="C159" t="inlineStr">
+        <is>
+          <t>12</t>
+        </is>
+      </c>
+      <c r="D159" t="inlineStr">
+        <is>
+          <t>help</t>
+        </is>
+      </c>
+      <c r="E159" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="160">
+      <c r="A160" t="n">
+        <v>0</v>
+      </c>
+      <c r="B160" t="n">
+        <v>2</v>
+      </c>
+      <c r="C160" t="inlineStr">
+        <is>
+          <t>13</t>
+        </is>
+      </c>
+      <c r="D160" t="inlineStr">
+        <is>
+          <t>sailors</t>
+        </is>
+      </c>
+      <c r="E160" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="161">
+      <c r="A161" t="n">
+        <v>0</v>
+      </c>
+      <c r="B161" t="n">
+        <v>2</v>
+      </c>
+      <c r="C161" t="inlineStr">
+        <is>
+          <t>14</t>
+        </is>
+      </c>
+      <c r="D161" t="inlineStr">
+        <is>
+          <t>find</t>
+        </is>
+      </c>
+      <c r="E161" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="162">
+      <c r="A162" t="n">
+        <v>0</v>
+      </c>
+      <c r="B162" t="n">
+        <v>2</v>
+      </c>
+      <c r="C162" t="inlineStr">
+        <is>
+          <t>15</t>
+        </is>
+      </c>
+      <c r="D162" t="inlineStr">
+        <is>
+          <t>their</t>
+        </is>
+      </c>
+      <c r="E162" t="inlineStr">
+        <is>
+          <t>O</t>
+        </is>
+      </c>
+    </row>
+    <row r="163">
+      <c r="A163" t="n">
+        <v>0</v>
+      </c>
+      <c r="B163" t="n">
+        <v>2</v>
+      </c>
+      <c r="C163" t="inlineStr">
+        <is>
+          <t>16</t>
+        </is>
+      </c>
+      <c r="D163" t="inlineStr">
         <is>
           <t>way</t>
         </is>
       </c>
-      <c r="E109" t="inlineStr">
+      <c r="E163" t="inlineStr">
         <is>
           <t>O</t>
         </is>

</xml_diff>